<commit_message>
class name change, database update
</commit_message>
<xml_diff>
--- a/Laptoptoimport.xlsx
+++ b/Laptoptoimport.xlsx
@@ -5,18 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\College Document\Web 2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\laptopwebsite\Web-2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6A8DA4CB-6944-4B1B-8820-4096377212C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32AE877F-CA68-4E22-866A-B373CD2338D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{349A10E7-D129-46A0-B31B-2131A9224112}"/>
+    <workbookView xWindow="5604" yWindow="1968" windowWidth="17436" windowHeight="9216" xr2:uid="{349A10E7-D129-46A0-B31B-2131A9224112}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="57">
   <si>
     <t>Tên laptop</t>
   </si>
@@ -64,24 +63,15 @@
     <t>CÂN NẶNG</t>
   </si>
   <si>
-    <t>DÒNG MÔ TẢ</t>
-  </si>
-  <si>
     <t>Asus ROG Zephyrus G15 GA503RM</t>
   </si>
   <si>
     <t>28.890.000</t>
   </si>
   <si>
-    <t>Ryzen 9-6900HS</t>
-  </si>
-  <si>
     <t>Asus</t>
   </si>
   <si>
-    <t>16GB</t>
-  </si>
-  <si>
     <t>512GB</t>
   </si>
   <si>
@@ -94,28 +84,127 @@
     <t>26.890.000</t>
   </si>
   <si>
-    <t>Ryzen 7-7735HS</t>
-  </si>
-  <si>
-    <t>RTX 4050</t>
-  </si>
-  <si>
     <t>1.7kg</t>
   </si>
   <si>
     <t xml:space="preserve"> Asus Zenbook 14X OLED Q420VA</t>
   </si>
   <si>
-    <t>Core i7-13700H</t>
-  </si>
-  <si>
     <t>20.890.000</t>
   </si>
   <si>
     <t xml:space="preserve">Iris Xe </t>
   </si>
   <si>
-    <t>Nvidia - RTX 3060 6GB</t>
+    <t xml:space="preserve"> ASUS TUF Gaming A15 FA507UV</t>
+  </si>
+  <si>
+    <t>32.990.000</t>
+  </si>
+  <si>
+    <t>1.6kg</t>
+  </si>
+  <si>
+    <t>2.2 kg</t>
+  </si>
+  <si>
+    <t>Kích thước màn hình</t>
+  </si>
+  <si>
+    <t>15.6"</t>
+  </si>
+  <si>
+    <t>14"</t>
+  </si>
+  <si>
+    <t>Độ phân giải</t>
+  </si>
+  <si>
+    <t>QHD+ (2560 x 1440) 16:9</t>
+  </si>
+  <si>
+    <t>2K+  (2560 x 1600) 16:10</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2.8K (2880 x 1800) 16:10 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">FHD (1920 x 1080) 16:9 </t>
+  </si>
+  <si>
+    <t>ASUS ROG Strix G16 G614JU</t>
+  </si>
+  <si>
+    <t>AMD Ryzen 9-6900HS</t>
+  </si>
+  <si>
+    <t>AMD Ryzen 7-7735HS</t>
+  </si>
+  <si>
+    <t>Intel Core i7-13700H</t>
+  </si>
+  <si>
+    <t>AMD Ryzen 9-8945H</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Intel Core i5-13450HX </t>
+  </si>
+  <si>
+    <t>30.990.000</t>
+  </si>
+  <si>
+    <t>Nhu Cầu</t>
+  </si>
+  <si>
+    <t>Gaming</t>
+  </si>
+  <si>
+    <t>Văn phòng</t>
+  </si>
+  <si>
+    <t>ASUS ProArt Studiobook 16 OLED W7600Z3A</t>
+  </si>
+  <si>
+    <t>76.990.000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Intel Core i9-12900H </t>
+  </si>
+  <si>
+    <t>8GB (1x8GB) DDR5 4800MHz</t>
+  </si>
+  <si>
+    <t>16GB (2x8GB) DDR5 4800MHz</t>
+  </si>
+  <si>
+    <t>16GB (1x16) LPDDR5 4800MHz</t>
+  </si>
+  <si>
+    <t>16GB  (2x8GB) DDR5 4800MHz</t>
+  </si>
+  <si>
+    <t>2.5 kg</t>
+  </si>
+  <si>
+    <t>16"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NVIDIA RTX A3000 12GB </t>
+  </si>
+  <si>
+    <t xml:space="preserve">	32GB (16x2) DDR5 4800MHz</t>
+  </si>
+  <si>
+    <t>FHD+  (1920 x 1200) 16:10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NVIDIA RTX 4060 8GB </t>
+  </si>
+  <si>
+    <t xml:space="preserve">NVIDIA RTX 4050 6GB </t>
+  </si>
+  <si>
+    <t>NVIDIA RTX 3060 6GB</t>
   </si>
 </sst>
 </file>
@@ -470,15 +559,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{221C85DB-D223-4886-A479-E6FFD04A93C4}">
-  <dimension ref="A1:AB14"/>
+  <dimension ref="A1:AN14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10:L10"/>
+    <sheetView tabSelected="1" topLeftCell="AC1" workbookViewId="0">
+      <selection activeCell="AD7" sqref="AD7:AE7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -503,34 +592,50 @@
         <v>1</v>
       </c>
       <c r="N1" s="1"/>
-      <c r="O1" s="1" t="s">
+      <c r="O1" s="1"/>
+      <c r="P1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="P1" s="1"/>
       <c r="Q1" s="1"/>
       <c r="R1" s="1"/>
-      <c r="S1" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="S1" s="1"/>
       <c r="T1" s="1"/>
       <c r="U1" s="1"/>
-      <c r="V1" s="1"/>
-      <c r="W1" s="1" t="s">
+      <c r="V1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="W1" s="1"/>
+      <c r="X1" s="1"/>
+      <c r="Y1" s="1"/>
+      <c r="Z1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="X1" s="1"/>
-      <c r="Y1" s="1" t="s">
+      <c r="AA1" s="1"/>
+      <c r="AB1" s="1"/>
+      <c r="AC1" s="1"/>
+      <c r="AD1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="Z1" s="1"/>
-      <c r="AA1" s="1" t="s">
+      <c r="AE1" s="1"/>
+      <c r="AF1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="AG1" s="1"/>
+      <c r="AH1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AI1" s="1"/>
+      <c r="AJ1" s="1"/>
+      <c r="AK1" s="1"/>
+      <c r="AL1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AM1" s="1"/>
+      <c r="AN1" s="1"/>
+    </row>
+    <row r="2" spans="1:40" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="AB1" s="1"/>
-    </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>10</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -542,43 +647,61 @@
       </c>
       <c r="H2" s="1"/>
       <c r="I2" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J2" s="1"/>
       <c r="K2" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="L2" s="1"/>
       <c r="M2" s="1" t="s">
-        <v>12</v>
+        <v>33</v>
       </c>
       <c r="N2" s="1"/>
-      <c r="O2" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="P2" s="1"/>
+      <c r="O2" s="1"/>
+      <c r="P2" s="1" t="s">
+        <v>56</v>
+      </c>
       <c r="Q2" s="1"/>
       <c r="R2" s="1"/>
-      <c r="S2" s="1" t="s">
-        <v>14</v>
-      </c>
+      <c r="S2" s="1"/>
       <c r="T2" s="1"/>
       <c r="U2" s="1"/>
-      <c r="V2" s="1"/>
-      <c r="W2" s="1" t="s">
-        <v>15</v>
-      </c>
+      <c r="V2" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="W2" s="1"/>
       <c r="X2" s="1"/>
-      <c r="Y2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="Z2" s="1"/>
+      <c r="Y2" s="1"/>
+      <c r="Z2" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="AA2" s="1"/>
       <c r="AB2" s="1"/>
+      <c r="AC2" s="1"/>
+      <c r="AD2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="AE2" s="1"/>
+      <c r="AF2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AG2" s="1"/>
+      <c r="AH2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AI2" s="1"/>
+      <c r="AJ2" s="1"/>
+      <c r="AK2" s="1"/>
+      <c r="AL2" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AM2" s="1"/>
+      <c r="AN2" s="1"/>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -590,43 +713,61 @@
       </c>
       <c r="H3" s="1"/>
       <c r="I3" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="J3" s="1"/>
       <c r="K3" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="L3" s="1"/>
       <c r="M3" s="1" t="s">
-        <v>19</v>
+        <v>34</v>
       </c>
       <c r="N3" s="1"/>
-      <c r="O3" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="P3" s="1"/>
+      <c r="O3" s="1"/>
+      <c r="P3" s="1" t="s">
+        <v>55</v>
+      </c>
       <c r="Q3" s="1"/>
       <c r="R3" s="1"/>
-      <c r="S3" s="1" t="s">
-        <v>14</v>
-      </c>
+      <c r="S3" s="1"/>
       <c r="T3" s="1"/>
       <c r="U3" s="1"/>
-      <c r="V3" s="1"/>
-      <c r="W3" s="1" t="s">
-        <v>15</v>
-      </c>
+      <c r="V3" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="W3" s="1"/>
       <c r="X3" s="1"/>
-      <c r="Y3" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="Z3" s="1"/>
+      <c r="Y3" s="1"/>
+      <c r="Z3" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="AA3" s="1"/>
       <c r="AB3" s="1"/>
+      <c r="AC3" s="1"/>
+      <c r="AD3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AE3" s="1"/>
+      <c r="AF3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AG3" s="1"/>
+      <c r="AH3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AI3" s="1"/>
+      <c r="AJ3" s="1"/>
+      <c r="AK3" s="1"/>
+      <c r="AL3" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AM3" s="1"/>
+      <c r="AN3" s="1"/>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -638,131 +779,251 @@
       </c>
       <c r="H4" s="1"/>
       <c r="I4" s="1" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="J4" s="1"/>
       <c r="K4" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="L4" s="1"/>
       <c r="M4" s="1" t="s">
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="N4" s="1"/>
-      <c r="O4" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="P4" s="1"/>
+      <c r="O4" s="1"/>
+      <c r="P4" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="Q4" s="1"/>
       <c r="R4" s="1"/>
       <c r="S4" s="1"/>
       <c r="T4" s="1"/>
       <c r="U4" s="1"/>
-      <c r="V4" s="1"/>
+      <c r="V4" s="1" t="s">
+        <v>47</v>
+      </c>
       <c r="W4" s="1"/>
       <c r="X4" s="1"/>
       <c r="Y4" s="1"/>
-      <c r="Z4" s="1"/>
+      <c r="Z4" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="AA4" s="1"/>
       <c r="AB4" s="1"/>
+      <c r="AC4" s="1"/>
+      <c r="AD4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="AE4" s="1"/>
+      <c r="AF4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AG4" s="1"/>
+      <c r="AH4" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AI4" s="1"/>
+      <c r="AJ4" s="1"/>
+      <c r="AK4" s="1"/>
+      <c r="AL4" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AM4" s="1"/>
+      <c r="AN4" s="1"/>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="A5" s="1"/>
+    <row r="5" spans="1:40" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
+      <c r="G5" s="1">
+        <v>65</v>
+      </c>
       <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
+      <c r="I5" s="1" t="s">
+        <v>21</v>
+      </c>
       <c r="J5" s="1"/>
       <c r="K5" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="L5" s="1"/>
-      <c r="M5" s="1"/>
+      <c r="M5" s="1" t="s">
+        <v>36</v>
+      </c>
       <c r="N5" s="1"/>
       <c r="O5" s="1"/>
-      <c r="P5" s="1"/>
+      <c r="P5" s="1" t="s">
+        <v>54</v>
+      </c>
       <c r="Q5" s="1"/>
       <c r="R5" s="1"/>
       <c r="S5" s="1"/>
       <c r="T5" s="1"/>
       <c r="U5" s="1"/>
-      <c r="V5" s="1"/>
+      <c r="V5" s="1" t="s">
+        <v>46</v>
+      </c>
       <c r="W5" s="1"/>
       <c r="X5" s="1"/>
       <c r="Y5" s="1"/>
-      <c r="Z5" s="1"/>
+      <c r="Z5" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="AA5" s="1"/>
       <c r="AB5" s="1"/>
+      <c r="AC5" s="1"/>
+      <c r="AD5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="AE5" s="1"/>
+      <c r="AF5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AG5" s="1"/>
+      <c r="AH5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AI5" s="1"/>
+      <c r="AJ5" s="1"/>
+      <c r="AK5" s="1"/>
+      <c r="AL5" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AM5" s="1"/>
+      <c r="AN5" s="1"/>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="A6" s="1"/>
+    <row r="6" spans="1:40" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>32</v>
+      </c>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
+      <c r="G6" s="1">
+        <v>20</v>
+      </c>
       <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
+      <c r="I6" s="1" t="s">
+        <v>38</v>
+      </c>
       <c r="J6" s="1"/>
       <c r="K6" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="L6" s="1"/>
-      <c r="M6" s="1"/>
+      <c r="M6" s="1" t="s">
+        <v>37</v>
+      </c>
       <c r="N6" s="1"/>
       <c r="O6" s="1"/>
-      <c r="P6" s="1"/>
+      <c r="P6" s="1" t="s">
+        <v>55</v>
+      </c>
       <c r="Q6" s="1"/>
       <c r="R6" s="1"/>
       <c r="S6" s="1"/>
       <c r="T6" s="1"/>
       <c r="U6" s="1"/>
-      <c r="V6" s="1"/>
+      <c r="V6" s="1" t="s">
+        <v>45</v>
+      </c>
       <c r="W6" s="1"/>
       <c r="X6" s="1"/>
       <c r="Y6" s="1"/>
-      <c r="Z6" s="1"/>
+      <c r="Z6" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="AA6" s="1"/>
       <c r="AB6" s="1"/>
+      <c r="AC6" s="1"/>
+      <c r="AD6" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AE6" s="1"/>
+      <c r="AF6" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="AG6" s="1"/>
+      <c r="AH6" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="AI6" s="1"/>
+      <c r="AJ6" s="1"/>
+      <c r="AK6" s="1"/>
+      <c r="AL6" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AM6" s="1"/>
+      <c r="AN6" s="1"/>
     </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="A7" s="1"/>
+    <row r="7" spans="1:40" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>42</v>
+      </c>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
+      <c r="G7" s="1">
+        <v>5</v>
+      </c>
       <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
+      <c r="I7" s="1" t="s">
+        <v>43</v>
+      </c>
       <c r="J7" s="1"/>
       <c r="K7" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="L7" s="1"/>
-      <c r="M7" s="1"/>
+      <c r="M7" s="1" t="s">
+        <v>44</v>
+      </c>
       <c r="N7" s="1"/>
       <c r="O7" s="1"/>
-      <c r="P7" s="1"/>
+      <c r="P7" s="1" t="s">
+        <v>51</v>
+      </c>
       <c r="Q7" s="1"/>
       <c r="R7" s="1"/>
       <c r="S7" s="1"/>
       <c r="T7" s="1"/>
       <c r="U7" s="1"/>
-      <c r="V7" s="1"/>
+      <c r="V7" s="1" t="s">
+        <v>52</v>
+      </c>
       <c r="W7" s="1"/>
       <c r="X7" s="1"/>
       <c r="Y7" s="1"/>
-      <c r="Z7" s="1"/>
+      <c r="Z7" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="AA7" s="1"/>
       <c r="AB7" s="1"/>
+      <c r="AC7" s="1"/>
+      <c r="AD7" s="1"/>
+      <c r="AE7" s="1"/>
+      <c r="AF7" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AG7" s="1"/>
+      <c r="AH7" s="1"/>
+      <c r="AI7" s="1"/>
+      <c r="AJ7" s="1"/>
+      <c r="AK7" s="1"/>
+      <c r="AL7" s="1"/>
+      <c r="AM7" s="1"/>
+      <c r="AN7" s="1"/>
     </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -788,11 +1049,27 @@
       <c r="W8" s="1"/>
       <c r="X8" s="1"/>
       <c r="Y8" s="1"/>
-      <c r="Z8" s="1"/>
+      <c r="Z8" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="AA8" s="1"/>
       <c r="AB8" s="1"/>
+      <c r="AC8" s="1"/>
+      <c r="AD8" s="1"/>
+      <c r="AE8" s="1"/>
+      <c r="AF8" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AG8" s="1"/>
+      <c r="AH8" s="1"/>
+      <c r="AI8" s="1"/>
+      <c r="AJ8" s="1"/>
+      <c r="AK8" s="1"/>
+      <c r="AL8" s="1"/>
+      <c r="AM8" s="1"/>
+      <c r="AN8" s="1"/>
     </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -818,11 +1095,27 @@
       <c r="W9" s="1"/>
       <c r="X9" s="1"/>
       <c r="Y9" s="1"/>
-      <c r="Z9" s="1"/>
+      <c r="Z9" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="AA9" s="1"/>
       <c r="AB9" s="1"/>
+      <c r="AC9" s="1"/>
+      <c r="AD9" s="1"/>
+      <c r="AE9" s="1"/>
+      <c r="AF9" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AG9" s="1"/>
+      <c r="AH9" s="1"/>
+      <c r="AI9" s="1"/>
+      <c r="AJ9" s="1"/>
+      <c r="AK9" s="1"/>
+      <c r="AL9" s="1"/>
+      <c r="AM9" s="1"/>
+      <c r="AN9" s="1"/>
     </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -848,11 +1141,27 @@
       <c r="W10" s="1"/>
       <c r="X10" s="1"/>
       <c r="Y10" s="1"/>
-      <c r="Z10" s="1"/>
+      <c r="Z10" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="AA10" s="1"/>
       <c r="AB10" s="1"/>
+      <c r="AC10" s="1"/>
+      <c r="AD10" s="1"/>
+      <c r="AE10" s="1"/>
+      <c r="AF10" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AG10" s="1"/>
+      <c r="AH10" s="1"/>
+      <c r="AI10" s="1"/>
+      <c r="AJ10" s="1"/>
+      <c r="AK10" s="1"/>
+      <c r="AL10" s="1"/>
+      <c r="AM10" s="1"/>
+      <c r="AN10" s="1"/>
     </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -878,11 +1187,27 @@
       <c r="W11" s="1"/>
       <c r="X11" s="1"/>
       <c r="Y11" s="1"/>
-      <c r="Z11" s="1"/>
+      <c r="Z11" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="AA11" s="1"/>
       <c r="AB11" s="1"/>
+      <c r="AC11" s="1"/>
+      <c r="AD11" s="1"/>
+      <c r="AE11" s="1"/>
+      <c r="AF11" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AG11" s="1"/>
+      <c r="AH11" s="1"/>
+      <c r="AI11" s="1"/>
+      <c r="AJ11" s="1"/>
+      <c r="AK11" s="1"/>
+      <c r="AL11" s="1"/>
+      <c r="AM11" s="1"/>
+      <c r="AN11" s="1"/>
     </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -908,11 +1233,27 @@
       <c r="W12" s="1"/>
       <c r="X12" s="1"/>
       <c r="Y12" s="1"/>
-      <c r="Z12" s="1"/>
+      <c r="Z12" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="AA12" s="1"/>
       <c r="AB12" s="1"/>
+      <c r="AC12" s="1"/>
+      <c r="AD12" s="1"/>
+      <c r="AE12" s="1"/>
+      <c r="AF12" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AG12" s="1"/>
+      <c r="AH12" s="1"/>
+      <c r="AI12" s="1"/>
+      <c r="AJ12" s="1"/>
+      <c r="AK12" s="1"/>
+      <c r="AL12" s="1"/>
+      <c r="AM12" s="1"/>
+      <c r="AN12" s="1"/>
     </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -938,11 +1279,27 @@
       <c r="W13" s="1"/>
       <c r="X13" s="1"/>
       <c r="Y13" s="1"/>
-      <c r="Z13" s="1"/>
+      <c r="Z13" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="AA13" s="1"/>
       <c r="AB13" s="1"/>
+      <c r="AC13" s="1"/>
+      <c r="AD13" s="1"/>
+      <c r="AE13" s="1"/>
+      <c r="AF13" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AG13" s="1"/>
+      <c r="AH13" s="1"/>
+      <c r="AI13" s="1"/>
+      <c r="AJ13" s="1"/>
+      <c r="AK13" s="1"/>
+      <c r="AL13" s="1"/>
+      <c r="AM13" s="1"/>
+      <c r="AN13" s="1"/>
     </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -968,41 +1325,147 @@
       <c r="W14" s="1"/>
       <c r="X14" s="1"/>
       <c r="Y14" s="1"/>
-      <c r="Z14" s="1"/>
+      <c r="Z14" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="AA14" s="1"/>
       <c r="AB14" s="1"/>
+      <c r="AC14" s="1"/>
+      <c r="AD14" s="1"/>
+      <c r="AE14" s="1"/>
+      <c r="AF14" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AG14" s="1"/>
+      <c r="AH14" s="1"/>
+      <c r="AI14" s="1"/>
+      <c r="AJ14" s="1"/>
+      <c r="AK14" s="1"/>
+      <c r="AL14" s="1"/>
+      <c r="AM14" s="1"/>
+      <c r="AN14" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="140">
-    <mergeCell ref="W1:X1"/>
-    <mergeCell ref="Y1:Z1"/>
-    <mergeCell ref="AA1:AB1"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A2:F2"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="I1:J1"/>
-    <mergeCell ref="K1:L1"/>
-    <mergeCell ref="M1:N1"/>
-    <mergeCell ref="O1:R1"/>
-    <mergeCell ref="O2:R2"/>
-    <mergeCell ref="S1:V1"/>
-    <mergeCell ref="S2:V2"/>
-    <mergeCell ref="A7:F7"/>
-    <mergeCell ref="A8:F8"/>
-    <mergeCell ref="A9:F9"/>
-    <mergeCell ref="A10:F10"/>
-    <mergeCell ref="A11:F11"/>
-    <mergeCell ref="A12:F12"/>
-    <mergeCell ref="A13:F13"/>
-    <mergeCell ref="A14:F14"/>
-    <mergeCell ref="A3:F3"/>
-    <mergeCell ref="A4:F4"/>
-    <mergeCell ref="A5:F5"/>
-    <mergeCell ref="A6:F6"/>
+  <mergeCells count="168">
+    <mergeCell ref="AH12:AK12"/>
+    <mergeCell ref="AH13:AK13"/>
+    <mergeCell ref="AH14:AK14"/>
+    <mergeCell ref="AL1:AN1"/>
+    <mergeCell ref="AL2:AN2"/>
+    <mergeCell ref="AL3:AN3"/>
+    <mergeCell ref="AL4:AN4"/>
+    <mergeCell ref="AL5:AN5"/>
+    <mergeCell ref="AL6:AN6"/>
+    <mergeCell ref="AL7:AN7"/>
+    <mergeCell ref="AL8:AN8"/>
+    <mergeCell ref="AL9:AN9"/>
+    <mergeCell ref="AL10:AN10"/>
+    <mergeCell ref="AL11:AN11"/>
+    <mergeCell ref="AL12:AN12"/>
+    <mergeCell ref="AL13:AN13"/>
+    <mergeCell ref="AL14:AN14"/>
+    <mergeCell ref="AH3:AK3"/>
+    <mergeCell ref="AH4:AK4"/>
+    <mergeCell ref="AH5:AK5"/>
+    <mergeCell ref="AH6:AK6"/>
+    <mergeCell ref="AH7:AK7"/>
+    <mergeCell ref="AH8:AK8"/>
+    <mergeCell ref="AH9:AK9"/>
+    <mergeCell ref="AH10:AK10"/>
+    <mergeCell ref="AH11:AK11"/>
+    <mergeCell ref="P7:U7"/>
+    <mergeCell ref="P8:U8"/>
+    <mergeCell ref="P9:U9"/>
+    <mergeCell ref="P10:U10"/>
+    <mergeCell ref="P11:U11"/>
+    <mergeCell ref="P12:U12"/>
+    <mergeCell ref="P13:U13"/>
+    <mergeCell ref="P14:U14"/>
+    <mergeCell ref="Z2:AC2"/>
+    <mergeCell ref="Z3:AC3"/>
+    <mergeCell ref="Z4:AC4"/>
+    <mergeCell ref="Z5:AC5"/>
+    <mergeCell ref="Z6:AC6"/>
+    <mergeCell ref="Z7:AC7"/>
+    <mergeCell ref="Z8:AC8"/>
+    <mergeCell ref="Z9:AC9"/>
+    <mergeCell ref="Z10:AC10"/>
+    <mergeCell ref="Z11:AC11"/>
+    <mergeCell ref="Z12:AC12"/>
+    <mergeCell ref="Z13:AC13"/>
+    <mergeCell ref="Z14:AC14"/>
+    <mergeCell ref="AF9:AG9"/>
+    <mergeCell ref="AF10:AG10"/>
+    <mergeCell ref="AF11:AG11"/>
+    <mergeCell ref="AF12:AG12"/>
+    <mergeCell ref="AF13:AG13"/>
+    <mergeCell ref="AF14:AG14"/>
+    <mergeCell ref="AF3:AG3"/>
+    <mergeCell ref="AF4:AG4"/>
+    <mergeCell ref="AF5:AG5"/>
+    <mergeCell ref="AF6:AG6"/>
+    <mergeCell ref="AF7:AG7"/>
+    <mergeCell ref="AF8:AG8"/>
+    <mergeCell ref="AD9:AE9"/>
+    <mergeCell ref="AD10:AE10"/>
+    <mergeCell ref="AD11:AE11"/>
+    <mergeCell ref="AD12:AE12"/>
+    <mergeCell ref="AD13:AE13"/>
+    <mergeCell ref="AD14:AE14"/>
+    <mergeCell ref="AD3:AE3"/>
+    <mergeCell ref="AD4:AE4"/>
+    <mergeCell ref="AD5:AE5"/>
+    <mergeCell ref="AD6:AE6"/>
+    <mergeCell ref="AD7:AE7"/>
+    <mergeCell ref="AD8:AE8"/>
+    <mergeCell ref="M14:O14"/>
+    <mergeCell ref="K11:L11"/>
+    <mergeCell ref="K12:L12"/>
+    <mergeCell ref="K13:L13"/>
+    <mergeCell ref="K14:L14"/>
+    <mergeCell ref="K9:L9"/>
+    <mergeCell ref="K10:L10"/>
+    <mergeCell ref="V3:Y3"/>
+    <mergeCell ref="V4:Y4"/>
+    <mergeCell ref="V5:Y5"/>
+    <mergeCell ref="V6:Y6"/>
+    <mergeCell ref="V7:Y7"/>
+    <mergeCell ref="V8:Y8"/>
+    <mergeCell ref="V9:Y9"/>
+    <mergeCell ref="V10:Y10"/>
+    <mergeCell ref="V11:Y11"/>
+    <mergeCell ref="V12:Y12"/>
+    <mergeCell ref="V13:Y13"/>
+    <mergeCell ref="V14:Y14"/>
+    <mergeCell ref="P3:U3"/>
+    <mergeCell ref="P4:U4"/>
+    <mergeCell ref="P5:U5"/>
+    <mergeCell ref="P6:U6"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="K6:L6"/>
+    <mergeCell ref="K7:L7"/>
+    <mergeCell ref="K8:L8"/>
+    <mergeCell ref="M9:O9"/>
+    <mergeCell ref="M10:O10"/>
+    <mergeCell ref="M11:O11"/>
+    <mergeCell ref="M12:O12"/>
+    <mergeCell ref="M13:O13"/>
+    <mergeCell ref="I9:J9"/>
+    <mergeCell ref="I10:J10"/>
+    <mergeCell ref="I11:J11"/>
+    <mergeCell ref="I12:J12"/>
+    <mergeCell ref="I13:J13"/>
+    <mergeCell ref="I14:J14"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="I4:J4"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="K4:L4"/>
+    <mergeCell ref="M3:O3"/>
+    <mergeCell ref="M4:O4"/>
     <mergeCell ref="G14:H14"/>
     <mergeCell ref="I2:J2"/>
     <mergeCell ref="K2:L2"/>
-    <mergeCell ref="M2:N2"/>
+    <mergeCell ref="M2:O2"/>
     <mergeCell ref="I5:J5"/>
     <mergeCell ref="I6:J6"/>
     <mergeCell ref="I7:J7"/>
@@ -1019,101 +1482,39 @@
     <mergeCell ref="G5:H5"/>
     <mergeCell ref="G6:H6"/>
     <mergeCell ref="G7:H7"/>
-    <mergeCell ref="O3:R3"/>
-    <mergeCell ref="O4:R4"/>
-    <mergeCell ref="I9:J9"/>
-    <mergeCell ref="I10:J10"/>
-    <mergeCell ref="I11:J11"/>
-    <mergeCell ref="I12:J12"/>
-    <mergeCell ref="I13:J13"/>
-    <mergeCell ref="I14:J14"/>
-    <mergeCell ref="W2:X2"/>
-    <mergeCell ref="Y2:Z2"/>
-    <mergeCell ref="AA2:AB2"/>
-    <mergeCell ref="I3:J3"/>
-    <mergeCell ref="I4:J4"/>
-    <mergeCell ref="K3:L3"/>
-    <mergeCell ref="K4:L4"/>
-    <mergeCell ref="O5:R5"/>
-    <mergeCell ref="O6:R6"/>
-    <mergeCell ref="O7:R7"/>
-    <mergeCell ref="O8:R8"/>
-    <mergeCell ref="O9:R9"/>
-    <mergeCell ref="O10:R10"/>
-    <mergeCell ref="O11:R11"/>
-    <mergeCell ref="O12:R12"/>
-    <mergeCell ref="O13:R13"/>
-    <mergeCell ref="M3:N3"/>
-    <mergeCell ref="M4:N4"/>
-    <mergeCell ref="M5:N5"/>
-    <mergeCell ref="M6:N6"/>
-    <mergeCell ref="M7:N7"/>
-    <mergeCell ref="M8:N8"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="K6:L6"/>
-    <mergeCell ref="K7:L7"/>
-    <mergeCell ref="K8:L8"/>
-    <mergeCell ref="M9:N9"/>
-    <mergeCell ref="M10:N10"/>
-    <mergeCell ref="M11:N11"/>
-    <mergeCell ref="M12:N12"/>
-    <mergeCell ref="M13:N13"/>
-    <mergeCell ref="M14:N14"/>
-    <mergeCell ref="K11:L11"/>
-    <mergeCell ref="K12:L12"/>
-    <mergeCell ref="K13:L13"/>
-    <mergeCell ref="K14:L14"/>
-    <mergeCell ref="K9:L9"/>
-    <mergeCell ref="K10:L10"/>
-    <mergeCell ref="S3:V3"/>
-    <mergeCell ref="S4:V4"/>
-    <mergeCell ref="S5:V5"/>
-    <mergeCell ref="S6:V6"/>
-    <mergeCell ref="S7:V7"/>
-    <mergeCell ref="S8:V8"/>
-    <mergeCell ref="O14:R14"/>
-    <mergeCell ref="S9:V9"/>
-    <mergeCell ref="S10:V10"/>
-    <mergeCell ref="S11:V11"/>
-    <mergeCell ref="S12:V12"/>
-    <mergeCell ref="S13:V13"/>
-    <mergeCell ref="S14:V14"/>
-    <mergeCell ref="W9:X9"/>
-    <mergeCell ref="W10:X10"/>
-    <mergeCell ref="W11:X11"/>
-    <mergeCell ref="W12:X12"/>
-    <mergeCell ref="W13:X13"/>
-    <mergeCell ref="W14:X14"/>
-    <mergeCell ref="W3:X3"/>
-    <mergeCell ref="W4:X4"/>
-    <mergeCell ref="W5:X5"/>
-    <mergeCell ref="W6:X6"/>
-    <mergeCell ref="W7:X7"/>
-    <mergeCell ref="W8:X8"/>
-    <mergeCell ref="Y9:Z9"/>
-    <mergeCell ref="Y10:Z10"/>
-    <mergeCell ref="Y11:Z11"/>
-    <mergeCell ref="Y12:Z12"/>
-    <mergeCell ref="Y13:Z13"/>
-    <mergeCell ref="Y14:Z14"/>
-    <mergeCell ref="Y3:Z3"/>
-    <mergeCell ref="Y4:Z4"/>
-    <mergeCell ref="Y5:Z5"/>
-    <mergeCell ref="Y6:Z6"/>
-    <mergeCell ref="Y7:Z7"/>
-    <mergeCell ref="Y8:Z8"/>
-    <mergeCell ref="AA9:AB9"/>
-    <mergeCell ref="AA10:AB10"/>
-    <mergeCell ref="AA11:AB11"/>
-    <mergeCell ref="AA12:AB12"/>
-    <mergeCell ref="AA13:AB13"/>
-    <mergeCell ref="AA14:AB14"/>
-    <mergeCell ref="AA3:AB3"/>
-    <mergeCell ref="AA4:AB4"/>
-    <mergeCell ref="AA5:AB5"/>
-    <mergeCell ref="AA6:AB6"/>
-    <mergeCell ref="AA7:AB7"/>
-    <mergeCell ref="AA8:AB8"/>
+    <mergeCell ref="M5:O5"/>
+    <mergeCell ref="M6:O6"/>
+    <mergeCell ref="M7:O7"/>
+    <mergeCell ref="M8:O8"/>
+    <mergeCell ref="A7:F7"/>
+    <mergeCell ref="A8:F8"/>
+    <mergeCell ref="A9:F9"/>
+    <mergeCell ref="A10:F10"/>
+    <mergeCell ref="A11:F11"/>
+    <mergeCell ref="A12:F12"/>
+    <mergeCell ref="A13:F13"/>
+    <mergeCell ref="A14:F14"/>
+    <mergeCell ref="A3:F3"/>
+    <mergeCell ref="A4:F4"/>
+    <mergeCell ref="A5:F5"/>
+    <mergeCell ref="A6:F6"/>
+    <mergeCell ref="AD1:AE1"/>
+    <mergeCell ref="AF1:AG1"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="I1:J1"/>
+    <mergeCell ref="K1:L1"/>
+    <mergeCell ref="M1:O1"/>
+    <mergeCell ref="V1:Y1"/>
+    <mergeCell ref="V2:Y2"/>
+    <mergeCell ref="AD2:AE2"/>
+    <mergeCell ref="AF2:AG2"/>
+    <mergeCell ref="P1:U1"/>
+    <mergeCell ref="P2:U2"/>
+    <mergeCell ref="Z1:AC1"/>
+    <mergeCell ref="AH1:AK1"/>
+    <mergeCell ref="AH2:AK2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
More data to import
</commit_message>
<xml_diff>
--- a/Laptoptoimport.xlsx
+++ b/Laptoptoimport.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\laptopwebsite\Web-2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32AE877F-CA68-4E22-866A-B373CD2338D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F03ECDA7-A3D4-4C67-AE2A-295D17DB7BB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5604" yWindow="1968" windowWidth="17436" windowHeight="9216" xr2:uid="{349A10E7-D129-46A0-B31B-2131A9224112}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{349A10E7-D129-46A0-B31B-2131A9224112}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="82">
   <si>
     <t>Tên laptop</t>
   </si>
@@ -93,9 +93,6 @@
     <t>20.890.000</t>
   </si>
   <si>
-    <t xml:space="preserve">Iris Xe </t>
-  </si>
-  <si>
     <t xml:space="preserve"> ASUS TUF Gaming A15 FA507UV</t>
   </si>
   <si>
@@ -159,9 +156,6 @@
     <t>Gaming</t>
   </si>
   <si>
-    <t>Văn phòng</t>
-  </si>
-  <si>
     <t>ASUS ProArt Studiobook 16 OLED W7600Z3A</t>
   </si>
   <si>
@@ -171,18 +165,6 @@
     <t xml:space="preserve">Intel Core i9-12900H </t>
   </si>
   <si>
-    <t>8GB (1x8GB) DDR5 4800MHz</t>
-  </si>
-  <si>
-    <t>16GB (2x8GB) DDR5 4800MHz</t>
-  </si>
-  <si>
-    <t>16GB (1x16) LPDDR5 4800MHz</t>
-  </si>
-  <si>
-    <t>16GB  (2x8GB) DDR5 4800MHz</t>
-  </si>
-  <si>
     <t>2.5 kg</t>
   </si>
   <si>
@@ -192,9 +174,6 @@
     <t xml:space="preserve">NVIDIA RTX A3000 12GB </t>
   </si>
   <si>
-    <t xml:space="preserve">	32GB (16x2) DDR5 4800MHz</t>
-  </si>
-  <si>
     <t>FHD+  (1920 x 1200) 16:10</t>
   </si>
   <si>
@@ -205,16 +184,118 @@
   </si>
   <si>
     <t>NVIDIA RTX 3060 6GB</t>
+  </si>
+  <si>
+    <t>1TB</t>
+  </si>
+  <si>
+    <t>2.4 kg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16” </t>
+  </si>
+  <si>
+    <t>4K (3840 x 2400)  16:10</t>
+  </si>
+  <si>
+    <t>Đô Hoạ</t>
+  </si>
+  <si>
+    <t>Văn Phòng</t>
+  </si>
+  <si>
+    <t>HP Envy X360 14es</t>
+  </si>
+  <si>
+    <t>15.490.000</t>
+  </si>
+  <si>
+    <t>HP</t>
+  </si>
+  <si>
+    <t>Intel Core i5-1335U</t>
+  </si>
+  <si>
+    <t>Intel Iris Xe</t>
+  </si>
+  <si>
+    <t>8GB DDR4 3200MHz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	32GB DDR5 4800MHz</t>
+  </si>
+  <si>
+    <t>8GB DDR5 4800MHz</t>
+  </si>
+  <si>
+    <t>16GB DDR5 4800MHz</t>
+  </si>
+  <si>
+    <t>16GB LPDDR5 4800MHz</t>
+  </si>
+  <si>
+    <t>1.52 kg</t>
+  </si>
+  <si>
+    <t>HP Pavilion 15</t>
+  </si>
+  <si>
+    <t>21.990.000</t>
+  </si>
+  <si>
+    <t>Intel Core i7-1255U</t>
+  </si>
+  <si>
+    <t>NVIDIA MX550 2GB</t>
+  </si>
+  <si>
+    <t>1.74 kg</t>
+  </si>
+  <si>
+    <t>HP Gaming Victus 15</t>
+  </si>
+  <si>
+    <t>15.990.000</t>
+  </si>
+  <si>
+    <t>NVIDIA RTX 2050 4GB</t>
+  </si>
+  <si>
+    <t>8GB DDR5 4800Mhz</t>
+  </si>
+  <si>
+    <t>2.3 kg</t>
+  </si>
+  <si>
+    <t>HP Probook 440 G9</t>
+  </si>
+  <si>
+    <t>23.490.000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AMD Ryzen 5-7535HS </t>
+  </si>
+  <si>
+    <t xml:space="preserve">16GB DDR4 3200 MHz </t>
+  </si>
+  <si>
+    <t>1.38 kg</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -561,8 +642,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{221C85DB-D223-4886-A479-E6FFD04A93C4}">
   <dimension ref="A1:AN14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AC1" workbookViewId="0">
-      <selection activeCell="AD7" sqref="AD7:AE7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12:F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -618,17 +699,17 @@
       </c>
       <c r="AE1" s="1"/>
       <c r="AF1" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="AG1" s="1"/>
       <c r="AH1" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="AI1" s="1"/>
       <c r="AJ1" s="1"/>
       <c r="AK1" s="1"/>
       <c r="AL1" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="AM1" s="1"/>
       <c r="AN1" s="1"/>
@@ -655,12 +736,12 @@
       </c>
       <c r="L2" s="1"/>
       <c r="M2" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="N2" s="1"/>
       <c r="O2" s="1"/>
       <c r="P2" s="1" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="Q2" s="1"/>
       <c r="R2" s="1"/>
@@ -668,7 +749,7 @@
       <c r="T2" s="1"/>
       <c r="U2" s="1"/>
       <c r="V2" s="1" t="s">
-        <v>48</v>
+        <v>64</v>
       </c>
       <c r="W2" s="1"/>
       <c r="X2" s="1"/>
@@ -684,17 +765,17 @@
       </c>
       <c r="AE2" s="1"/>
       <c r="AF2" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="AG2" s="1"/>
       <c r="AH2" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="AI2" s="1"/>
       <c r="AJ2" s="1"/>
       <c r="AK2" s="1"/>
       <c r="AL2" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="AM2" s="1"/>
       <c r="AN2" s="1"/>
@@ -721,12 +802,12 @@
       </c>
       <c r="L3" s="1"/>
       <c r="M3" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="N3" s="1"/>
       <c r="O3" s="1"/>
       <c r="P3" s="1" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="Q3" s="1"/>
       <c r="R3" s="1"/>
@@ -734,7 +815,7 @@
       <c r="T3" s="1"/>
       <c r="U3" s="1"/>
       <c r="V3" s="1" t="s">
-        <v>48</v>
+        <v>64</v>
       </c>
       <c r="W3" s="1"/>
       <c r="X3" s="1"/>
@@ -750,17 +831,17 @@
       </c>
       <c r="AE3" s="1"/>
       <c r="AF3" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="AG3" s="1"/>
       <c r="AH3" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="AI3" s="1"/>
       <c r="AJ3" s="1"/>
       <c r="AK3" s="1"/>
       <c r="AL3" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="AM3" s="1"/>
       <c r="AN3" s="1"/>
@@ -787,12 +868,12 @@
       </c>
       <c r="L4" s="1"/>
       <c r="M4" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="N4" s="1"/>
       <c r="O4" s="1"/>
       <c r="P4" s="1" t="s">
-        <v>19</v>
+        <v>60</v>
       </c>
       <c r="Q4" s="1"/>
       <c r="R4" s="1"/>
@@ -800,7 +881,7 @@
       <c r="T4" s="1"/>
       <c r="U4" s="1"/>
       <c r="V4" s="1" t="s">
-        <v>47</v>
+        <v>65</v>
       </c>
       <c r="W4" s="1"/>
       <c r="X4" s="1"/>
@@ -812,28 +893,28 @@
       <c r="AB4" s="1"/>
       <c r="AC4" s="1"/>
       <c r="AD4" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="AE4" s="1"/>
       <c r="AF4" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="AG4" s="1"/>
       <c r="AH4" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="AI4" s="1"/>
       <c r="AJ4" s="1"/>
       <c r="AK4" s="1"/>
       <c r="AL4" s="1" t="s">
-        <v>41</v>
+        <v>55</v>
       </c>
       <c r="AM4" s="1"/>
       <c r="AN4" s="1"/>
     </row>
     <row r="5" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -845,7 +926,7 @@
       </c>
       <c r="H5" s="1"/>
       <c r="I5" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J5" s="1"/>
       <c r="K5" s="1" t="s">
@@ -853,12 +934,12 @@
       </c>
       <c r="L5" s="1"/>
       <c r="M5" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="N5" s="1"/>
       <c r="O5" s="1"/>
       <c r="P5" s="1" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="Q5" s="1"/>
       <c r="R5" s="1"/>
@@ -866,7 +947,7 @@
       <c r="T5" s="1"/>
       <c r="U5" s="1"/>
       <c r="V5" s="1" t="s">
-        <v>46</v>
+        <v>64</v>
       </c>
       <c r="W5" s="1"/>
       <c r="X5" s="1"/>
@@ -878,28 +959,28 @@
       <c r="AB5" s="1"/>
       <c r="AC5" s="1"/>
       <c r="AD5" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="AE5" s="1"/>
       <c r="AF5" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="AG5" s="1"/>
       <c r="AH5" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="AI5" s="1"/>
       <c r="AJ5" s="1"/>
       <c r="AK5" s="1"/>
       <c r="AL5" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="AM5" s="1"/>
       <c r="AN5" s="1"/>
     </row>
     <row r="6" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -911,7 +992,7 @@
       </c>
       <c r="H6" s="1"/>
       <c r="I6" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J6" s="1"/>
       <c r="K6" s="1" t="s">
@@ -919,12 +1000,12 @@
       </c>
       <c r="L6" s="1"/>
       <c r="M6" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="N6" s="1"/>
       <c r="O6" s="1"/>
       <c r="P6" s="1" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="Q6" s="1"/>
       <c r="R6" s="1"/>
@@ -932,7 +1013,7 @@
       <c r="T6" s="1"/>
       <c r="U6" s="1"/>
       <c r="V6" s="1" t="s">
-        <v>45</v>
+        <v>63</v>
       </c>
       <c r="W6" s="1"/>
       <c r="X6" s="1"/>
@@ -944,28 +1025,28 @@
       <c r="AB6" s="1"/>
       <c r="AC6" s="1"/>
       <c r="AD6" s="1" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="AE6" s="1"/>
       <c r="AF6" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="AG6" s="1"/>
       <c r="AH6" s="1" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="AI6" s="1"/>
       <c r="AJ6" s="1"/>
       <c r="AK6" s="1"/>
       <c r="AL6" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="AM6" s="1"/>
       <c r="AN6" s="1"/>
     </row>
     <row r="7" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -977,7 +1058,7 @@
       </c>
       <c r="H7" s="1"/>
       <c r="I7" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="J7" s="1"/>
       <c r="K7" s="1" t="s">
@@ -985,12 +1066,12 @@
       </c>
       <c r="L7" s="1"/>
       <c r="M7" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="N7" s="1"/>
       <c r="O7" s="1"/>
       <c r="P7" s="1" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="Q7" s="1"/>
       <c r="R7" s="1"/>
@@ -998,54 +1079,74 @@
       <c r="T7" s="1"/>
       <c r="U7" s="1"/>
       <c r="V7" s="1" t="s">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="W7" s="1"/>
       <c r="X7" s="1"/>
       <c r="Y7" s="1"/>
       <c r="Z7" s="1" t="s">
-        <v>12</v>
+        <v>50</v>
       </c>
       <c r="AA7" s="1"/>
       <c r="AB7" s="1"/>
       <c r="AC7" s="1"/>
-      <c r="AD7" s="1"/>
+      <c r="AD7" s="1" t="s">
+        <v>51</v>
+      </c>
       <c r="AE7" s="1"/>
       <c r="AF7" s="1" t="s">
-        <v>25</v>
+        <v>52</v>
       </c>
       <c r="AG7" s="1"/>
-      <c r="AH7" s="1"/>
+      <c r="AH7" s="1" t="s">
+        <v>53</v>
+      </c>
       <c r="AI7" s="1"/>
       <c r="AJ7" s="1"/>
       <c r="AK7" s="1"/>
-      <c r="AL7" s="1"/>
+      <c r="AL7" s="1" t="s">
+        <v>54</v>
+      </c>
       <c r="AM7" s="1"/>
       <c r="AN7" s="1"/>
     </row>
     <row r="8" spans="1:40" x14ac:dyDescent="0.3">
-      <c r="A8" s="1"/>
+      <c r="A8" s="1" t="s">
+        <v>56</v>
+      </c>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
+      <c r="G8" s="1">
+        <v>24</v>
+      </c>
       <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
+      <c r="I8" s="1" t="s">
+        <v>57</v>
+      </c>
       <c r="J8" s="1"/>
-      <c r="K8" s="1"/>
+      <c r="K8" s="1" t="s">
+        <v>58</v>
+      </c>
       <c r="L8" s="1"/>
-      <c r="M8" s="1"/>
+      <c r="M8" s="1" t="s">
+        <v>59</v>
+      </c>
       <c r="N8" s="1"/>
       <c r="O8" s="1"/>
-      <c r="P8" s="1"/>
+      <c r="P8" s="1" t="s">
+        <v>60</v>
+      </c>
       <c r="Q8" s="1"/>
       <c r="R8" s="1"/>
       <c r="S8" s="1"/>
       <c r="T8" s="1"/>
       <c r="U8" s="1"/>
-      <c r="V8" s="1"/>
+      <c r="V8" s="1" t="s">
+        <v>61</v>
+      </c>
       <c r="W8" s="1"/>
       <c r="X8" s="1"/>
       <c r="Y8" s="1"/>
@@ -1055,43 +1156,63 @@
       <c r="AA8" s="1"/>
       <c r="AB8" s="1"/>
       <c r="AC8" s="1"/>
-      <c r="AD8" s="1"/>
+      <c r="AD8" s="1" t="s">
+        <v>66</v>
+      </c>
       <c r="AE8" s="1"/>
       <c r="AF8" s="1" t="s">
         <v>25</v>
       </c>
       <c r="AG8" s="1"/>
-      <c r="AH8" s="1"/>
+      <c r="AH8" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="AI8" s="1"/>
       <c r="AJ8" s="1"/>
       <c r="AK8" s="1"/>
-      <c r="AL8" s="1"/>
+      <c r="AL8" s="1" t="s">
+        <v>55</v>
+      </c>
       <c r="AM8" s="1"/>
       <c r="AN8" s="1"/>
     </row>
     <row r="9" spans="1:40" x14ac:dyDescent="0.3">
-      <c r="A9" s="1"/>
+      <c r="A9" s="1" t="s">
+        <v>67</v>
+      </c>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
+      <c r="G9" s="1">
+        <v>50</v>
+      </c>
       <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
+      <c r="I9" s="1" t="s">
+        <v>68</v>
+      </c>
       <c r="J9" s="1"/>
-      <c r="K9" s="1"/>
+      <c r="K9" s="1" t="s">
+        <v>58</v>
+      </c>
       <c r="L9" s="1"/>
-      <c r="M9" s="1"/>
+      <c r="M9" s="1" t="s">
+        <v>69</v>
+      </c>
       <c r="N9" s="1"/>
       <c r="O9" s="1"/>
-      <c r="P9" s="1"/>
+      <c r="P9" s="1" t="s">
+        <v>70</v>
+      </c>
       <c r="Q9" s="1"/>
       <c r="R9" s="1"/>
       <c r="S9" s="1"/>
       <c r="T9" s="1"/>
       <c r="U9" s="1"/>
-      <c r="V9" s="1"/>
+      <c r="V9" s="1" t="s">
+        <v>61</v>
+      </c>
       <c r="W9" s="1"/>
       <c r="X9" s="1"/>
       <c r="Y9" s="1"/>
@@ -1101,43 +1222,63 @@
       <c r="AA9" s="1"/>
       <c r="AB9" s="1"/>
       <c r="AC9" s="1"/>
-      <c r="AD9" s="1"/>
+      <c r="AD9" s="1" t="s">
+        <v>71</v>
+      </c>
       <c r="AE9" s="1"/>
       <c r="AF9" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="AG9" s="1"/>
-      <c r="AH9" s="1"/>
+      <c r="AH9" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="AI9" s="1"/>
       <c r="AJ9" s="1"/>
       <c r="AK9" s="1"/>
-      <c r="AL9" s="1"/>
+      <c r="AL9" s="1" t="s">
+        <v>55</v>
+      </c>
       <c r="AM9" s="1"/>
       <c r="AN9" s="1"/>
     </row>
     <row r="10" spans="1:40" x14ac:dyDescent="0.3">
-      <c r="A10" s="1"/>
+      <c r="A10" s="1" t="s">
+        <v>72</v>
+      </c>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
+      <c r="G10" s="1">
+        <v>32</v>
+      </c>
       <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
+      <c r="I10" s="1" t="s">
+        <v>73</v>
+      </c>
       <c r="J10" s="1"/>
-      <c r="K10" s="1"/>
+      <c r="K10" s="1" t="s">
+        <v>58</v>
+      </c>
       <c r="L10" s="1"/>
-      <c r="M10" s="1"/>
+      <c r="M10" s="1" t="s">
+        <v>79</v>
+      </c>
       <c r="N10" s="1"/>
       <c r="O10" s="1"/>
-      <c r="P10" s="1"/>
+      <c r="P10" s="1" t="s">
+        <v>74</v>
+      </c>
       <c r="Q10" s="1"/>
       <c r="R10" s="1"/>
       <c r="S10" s="1"/>
       <c r="T10" s="1"/>
       <c r="U10" s="1"/>
-      <c r="V10" s="1"/>
+      <c r="V10" s="1" t="s">
+        <v>75</v>
+      </c>
       <c r="W10" s="1"/>
       <c r="X10" s="1"/>
       <c r="Y10" s="1"/>
@@ -1147,43 +1288,63 @@
       <c r="AA10" s="1"/>
       <c r="AB10" s="1"/>
       <c r="AC10" s="1"/>
-      <c r="AD10" s="1"/>
+      <c r="AD10" s="1" t="s">
+        <v>76</v>
+      </c>
       <c r="AE10" s="1"/>
       <c r="AF10" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="AG10" s="1"/>
-      <c r="AH10" s="1"/>
+      <c r="AH10" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="AI10" s="1"/>
       <c r="AJ10" s="1"/>
       <c r="AK10" s="1"/>
-      <c r="AL10" s="1"/>
+      <c r="AL10" s="1" t="s">
+        <v>39</v>
+      </c>
       <c r="AM10" s="1"/>
       <c r="AN10" s="1"/>
     </row>
     <row r="11" spans="1:40" x14ac:dyDescent="0.3">
-      <c r="A11" s="1"/>
+      <c r="A11" s="1" t="s">
+        <v>77</v>
+      </c>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
+      <c r="G11" s="1">
+        <v>12</v>
+      </c>
       <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
+      <c r="I11" s="1" t="s">
+        <v>78</v>
+      </c>
       <c r="J11" s="1"/>
-      <c r="K11" s="1"/>
+      <c r="K11" s="1" t="s">
+        <v>58</v>
+      </c>
       <c r="L11" s="1"/>
-      <c r="M11" s="1"/>
+      <c r="M11" s="1" t="s">
+        <v>69</v>
+      </c>
       <c r="N11" s="1"/>
       <c r="O11" s="1"/>
-      <c r="P11" s="1"/>
+      <c r="P11" s="1" t="s">
+        <v>60</v>
+      </c>
       <c r="Q11" s="1"/>
       <c r="R11" s="1"/>
       <c r="S11" s="1"/>
       <c r="T11" s="1"/>
       <c r="U11" s="1"/>
-      <c r="V11" s="1"/>
+      <c r="V11" s="1" t="s">
+        <v>80</v>
+      </c>
       <c r="W11" s="1"/>
       <c r="X11" s="1"/>
       <c r="Y11" s="1"/>
@@ -1193,17 +1354,23 @@
       <c r="AA11" s="1"/>
       <c r="AB11" s="1"/>
       <c r="AC11" s="1"/>
-      <c r="AD11" s="1"/>
+      <c r="AD11" s="1" t="s">
+        <v>81</v>
+      </c>
       <c r="AE11" s="1"/>
       <c r="AF11" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="AG11" s="1"/>
-      <c r="AH11" s="1"/>
+      <c r="AH11" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="AI11" s="1"/>
       <c r="AJ11" s="1"/>
       <c r="AK11" s="1"/>
-      <c r="AL11" s="1"/>
+      <c r="AL11" s="1" t="s">
+        <v>55</v>
+      </c>
       <c r="AM11" s="1"/>
       <c r="AN11" s="1"/>
     </row>
@@ -1242,7 +1409,7 @@
       <c r="AD12" s="1"/>
       <c r="AE12" s="1"/>
       <c r="AF12" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="AG12" s="1"/>
       <c r="AH12" s="1"/>
@@ -1288,7 +1455,7 @@
       <c r="AD13" s="1"/>
       <c r="AE13" s="1"/>
       <c r="AF13" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="AG13" s="1"/>
       <c r="AH13" s="1"/>
@@ -1334,7 +1501,7 @@
       <c r="AD14" s="1"/>
       <c r="AE14" s="1"/>
       <c r="AF14" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="AG14" s="1"/>
       <c r="AH14" s="1"/>
@@ -1347,6 +1514,150 @@
     </row>
   </sheetData>
   <mergeCells count="168">
+    <mergeCell ref="AH1:AK1"/>
+    <mergeCell ref="AH2:AK2"/>
+    <mergeCell ref="AD1:AE1"/>
+    <mergeCell ref="AF1:AG1"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="I1:J1"/>
+    <mergeCell ref="K1:L1"/>
+    <mergeCell ref="M1:O1"/>
+    <mergeCell ref="V1:Y1"/>
+    <mergeCell ref="V2:Y2"/>
+    <mergeCell ref="AD2:AE2"/>
+    <mergeCell ref="AF2:AG2"/>
+    <mergeCell ref="P1:U1"/>
+    <mergeCell ref="P2:U2"/>
+    <mergeCell ref="Z1:AC1"/>
+    <mergeCell ref="A9:F9"/>
+    <mergeCell ref="A10:F10"/>
+    <mergeCell ref="A11:F11"/>
+    <mergeCell ref="A12:F12"/>
+    <mergeCell ref="A13:F13"/>
+    <mergeCell ref="A14:F14"/>
+    <mergeCell ref="A3:F3"/>
+    <mergeCell ref="A4:F4"/>
+    <mergeCell ref="A5:F5"/>
+    <mergeCell ref="A6:F6"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="M5:O5"/>
+    <mergeCell ref="M6:O6"/>
+    <mergeCell ref="M7:O7"/>
+    <mergeCell ref="M8:O8"/>
+    <mergeCell ref="A7:F7"/>
+    <mergeCell ref="A8:F8"/>
+    <mergeCell ref="I14:J14"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="I4:J4"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="K4:L4"/>
+    <mergeCell ref="M3:O3"/>
+    <mergeCell ref="M4:O4"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="M2:O2"/>
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="I6:J6"/>
+    <mergeCell ref="I7:J7"/>
+    <mergeCell ref="I8:J8"/>
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="K6:L6"/>
+    <mergeCell ref="K7:L7"/>
+    <mergeCell ref="K8:L8"/>
+    <mergeCell ref="M9:O9"/>
+    <mergeCell ref="M10:O10"/>
+    <mergeCell ref="M11:O11"/>
+    <mergeCell ref="M12:O12"/>
+    <mergeCell ref="M13:O13"/>
+    <mergeCell ref="I9:J9"/>
+    <mergeCell ref="I10:J10"/>
+    <mergeCell ref="I11:J11"/>
+    <mergeCell ref="I12:J12"/>
+    <mergeCell ref="I13:J13"/>
+    <mergeCell ref="M14:O14"/>
+    <mergeCell ref="K11:L11"/>
+    <mergeCell ref="K12:L12"/>
+    <mergeCell ref="K13:L13"/>
+    <mergeCell ref="K14:L14"/>
+    <mergeCell ref="K9:L9"/>
+    <mergeCell ref="K10:L10"/>
+    <mergeCell ref="V3:Y3"/>
+    <mergeCell ref="V4:Y4"/>
+    <mergeCell ref="V5:Y5"/>
+    <mergeCell ref="V6:Y6"/>
+    <mergeCell ref="V7:Y7"/>
+    <mergeCell ref="V8:Y8"/>
+    <mergeCell ref="V9:Y9"/>
+    <mergeCell ref="V10:Y10"/>
+    <mergeCell ref="V11:Y11"/>
+    <mergeCell ref="V12:Y12"/>
+    <mergeCell ref="V13:Y13"/>
+    <mergeCell ref="V14:Y14"/>
+    <mergeCell ref="P3:U3"/>
+    <mergeCell ref="P4:U4"/>
+    <mergeCell ref="P5:U5"/>
+    <mergeCell ref="P6:U6"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="AF14:AG14"/>
+    <mergeCell ref="AF3:AG3"/>
+    <mergeCell ref="AF4:AG4"/>
+    <mergeCell ref="AF5:AG5"/>
+    <mergeCell ref="AF6:AG6"/>
+    <mergeCell ref="AF7:AG7"/>
+    <mergeCell ref="AF8:AG8"/>
+    <mergeCell ref="AD9:AE9"/>
+    <mergeCell ref="AD10:AE10"/>
+    <mergeCell ref="AD11:AE11"/>
+    <mergeCell ref="AD12:AE12"/>
+    <mergeCell ref="AD13:AE13"/>
+    <mergeCell ref="AD14:AE14"/>
+    <mergeCell ref="AD3:AE3"/>
+    <mergeCell ref="AD4:AE4"/>
+    <mergeCell ref="AD5:AE5"/>
+    <mergeCell ref="AD6:AE6"/>
+    <mergeCell ref="AD7:AE7"/>
+    <mergeCell ref="AD8:AE8"/>
+    <mergeCell ref="P14:U14"/>
+    <mergeCell ref="Z2:AC2"/>
+    <mergeCell ref="Z3:AC3"/>
+    <mergeCell ref="Z4:AC4"/>
+    <mergeCell ref="Z5:AC5"/>
+    <mergeCell ref="Z6:AC6"/>
+    <mergeCell ref="Z7:AC7"/>
+    <mergeCell ref="Z8:AC8"/>
+    <mergeCell ref="Z9:AC9"/>
+    <mergeCell ref="Z10:AC10"/>
+    <mergeCell ref="Z11:AC11"/>
+    <mergeCell ref="Z12:AC12"/>
+    <mergeCell ref="Z13:AC13"/>
+    <mergeCell ref="Z14:AC14"/>
+    <mergeCell ref="AH10:AK10"/>
+    <mergeCell ref="AH11:AK11"/>
+    <mergeCell ref="P7:U7"/>
+    <mergeCell ref="P8:U8"/>
+    <mergeCell ref="P9:U9"/>
+    <mergeCell ref="P10:U10"/>
+    <mergeCell ref="P11:U11"/>
+    <mergeCell ref="P12:U12"/>
+    <mergeCell ref="P13:U13"/>
+    <mergeCell ref="AF9:AG9"/>
+    <mergeCell ref="AF10:AG10"/>
+    <mergeCell ref="AF11:AG11"/>
+    <mergeCell ref="AF12:AG12"/>
+    <mergeCell ref="AF13:AG13"/>
     <mergeCell ref="AH12:AK12"/>
     <mergeCell ref="AH13:AK13"/>
     <mergeCell ref="AH14:AK14"/>
@@ -1371,151 +1682,8 @@
     <mergeCell ref="AH7:AK7"/>
     <mergeCell ref="AH8:AK8"/>
     <mergeCell ref="AH9:AK9"/>
-    <mergeCell ref="AH10:AK10"/>
-    <mergeCell ref="AH11:AK11"/>
-    <mergeCell ref="P7:U7"/>
-    <mergeCell ref="P8:U8"/>
-    <mergeCell ref="P9:U9"/>
-    <mergeCell ref="P10:U10"/>
-    <mergeCell ref="P11:U11"/>
-    <mergeCell ref="P12:U12"/>
-    <mergeCell ref="P13:U13"/>
-    <mergeCell ref="P14:U14"/>
-    <mergeCell ref="Z2:AC2"/>
-    <mergeCell ref="Z3:AC3"/>
-    <mergeCell ref="Z4:AC4"/>
-    <mergeCell ref="Z5:AC5"/>
-    <mergeCell ref="Z6:AC6"/>
-    <mergeCell ref="Z7:AC7"/>
-    <mergeCell ref="Z8:AC8"/>
-    <mergeCell ref="Z9:AC9"/>
-    <mergeCell ref="Z10:AC10"/>
-    <mergeCell ref="Z11:AC11"/>
-    <mergeCell ref="Z12:AC12"/>
-    <mergeCell ref="Z13:AC13"/>
-    <mergeCell ref="Z14:AC14"/>
-    <mergeCell ref="AF9:AG9"/>
-    <mergeCell ref="AF10:AG10"/>
-    <mergeCell ref="AF11:AG11"/>
-    <mergeCell ref="AF12:AG12"/>
-    <mergeCell ref="AF13:AG13"/>
-    <mergeCell ref="AF14:AG14"/>
-    <mergeCell ref="AF3:AG3"/>
-    <mergeCell ref="AF4:AG4"/>
-    <mergeCell ref="AF5:AG5"/>
-    <mergeCell ref="AF6:AG6"/>
-    <mergeCell ref="AF7:AG7"/>
-    <mergeCell ref="AF8:AG8"/>
-    <mergeCell ref="AD9:AE9"/>
-    <mergeCell ref="AD10:AE10"/>
-    <mergeCell ref="AD11:AE11"/>
-    <mergeCell ref="AD12:AE12"/>
-    <mergeCell ref="AD13:AE13"/>
-    <mergeCell ref="AD14:AE14"/>
-    <mergeCell ref="AD3:AE3"/>
-    <mergeCell ref="AD4:AE4"/>
-    <mergeCell ref="AD5:AE5"/>
-    <mergeCell ref="AD6:AE6"/>
-    <mergeCell ref="AD7:AE7"/>
-    <mergeCell ref="AD8:AE8"/>
-    <mergeCell ref="M14:O14"/>
-    <mergeCell ref="K11:L11"/>
-    <mergeCell ref="K12:L12"/>
-    <mergeCell ref="K13:L13"/>
-    <mergeCell ref="K14:L14"/>
-    <mergeCell ref="K9:L9"/>
-    <mergeCell ref="K10:L10"/>
-    <mergeCell ref="V3:Y3"/>
-    <mergeCell ref="V4:Y4"/>
-    <mergeCell ref="V5:Y5"/>
-    <mergeCell ref="V6:Y6"/>
-    <mergeCell ref="V7:Y7"/>
-    <mergeCell ref="V8:Y8"/>
-    <mergeCell ref="V9:Y9"/>
-    <mergeCell ref="V10:Y10"/>
-    <mergeCell ref="V11:Y11"/>
-    <mergeCell ref="V12:Y12"/>
-    <mergeCell ref="V13:Y13"/>
-    <mergeCell ref="V14:Y14"/>
-    <mergeCell ref="P3:U3"/>
-    <mergeCell ref="P4:U4"/>
-    <mergeCell ref="P5:U5"/>
-    <mergeCell ref="P6:U6"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="K6:L6"/>
-    <mergeCell ref="K7:L7"/>
-    <mergeCell ref="K8:L8"/>
-    <mergeCell ref="M9:O9"/>
-    <mergeCell ref="M10:O10"/>
-    <mergeCell ref="M11:O11"/>
-    <mergeCell ref="M12:O12"/>
-    <mergeCell ref="M13:O13"/>
-    <mergeCell ref="I9:J9"/>
-    <mergeCell ref="I10:J10"/>
-    <mergeCell ref="I11:J11"/>
-    <mergeCell ref="I12:J12"/>
-    <mergeCell ref="I13:J13"/>
-    <mergeCell ref="I14:J14"/>
-    <mergeCell ref="I3:J3"/>
-    <mergeCell ref="I4:J4"/>
-    <mergeCell ref="K3:L3"/>
-    <mergeCell ref="K4:L4"/>
-    <mergeCell ref="M3:O3"/>
-    <mergeCell ref="M4:O4"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="I2:J2"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="M2:O2"/>
-    <mergeCell ref="I5:J5"/>
-    <mergeCell ref="I6:J6"/>
-    <mergeCell ref="I7:J7"/>
-    <mergeCell ref="I8:J8"/>
-    <mergeCell ref="G8:H8"/>
-    <mergeCell ref="G9:H9"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="G11:H11"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="G13:H13"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="M5:O5"/>
-    <mergeCell ref="M6:O6"/>
-    <mergeCell ref="M7:O7"/>
-    <mergeCell ref="M8:O8"/>
-    <mergeCell ref="A7:F7"/>
-    <mergeCell ref="A8:F8"/>
-    <mergeCell ref="A9:F9"/>
-    <mergeCell ref="A10:F10"/>
-    <mergeCell ref="A11:F11"/>
-    <mergeCell ref="A12:F12"/>
-    <mergeCell ref="A13:F13"/>
-    <mergeCell ref="A14:F14"/>
-    <mergeCell ref="A3:F3"/>
-    <mergeCell ref="A4:F4"/>
-    <mergeCell ref="A5:F5"/>
-    <mergeCell ref="A6:F6"/>
-    <mergeCell ref="AD1:AE1"/>
-    <mergeCell ref="AF1:AG1"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A2:F2"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="I1:J1"/>
-    <mergeCell ref="K1:L1"/>
-    <mergeCell ref="M1:O1"/>
-    <mergeCell ref="V1:Y1"/>
-    <mergeCell ref="V2:Y2"/>
-    <mergeCell ref="AD2:AE2"/>
-    <mergeCell ref="AF2:AG2"/>
-    <mergeCell ref="P1:U1"/>
-    <mergeCell ref="P2:U2"/>
-    <mergeCell ref="Z1:AC1"/>
-    <mergeCell ref="AH1:AK1"/>
-    <mergeCell ref="AH2:AK2"/>
   </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>